<commit_message>
Adjusting the NRG location
</commit_message>
<xml_diff>
--- a/data_fetching/Entsoe/Actual_Production_Solar.xlsx
+++ b/data_fetching/Entsoe/Actual_Production_Solar.xlsx
@@ -397,7 +397,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>45946.01041666666</v>
+        <v>45947.01041666666</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -405,7 +405,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>45946.02083333334</v>
+        <v>45947.02083333334</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -413,7 +413,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>45946.03125</v>
+        <v>45947.03125</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -421,7 +421,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>45946.04166666666</v>
+        <v>45947.04166666666</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -429,7 +429,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>45946.05208333334</v>
+        <v>45947.05208333334</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -437,7 +437,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>45946.0625</v>
+        <v>45947.0625</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -445,7 +445,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>45946.07291666666</v>
+        <v>45947.07291666666</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>45946.08333333334</v>
+        <v>45947.08333333334</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>45946.09375</v>
+        <v>45947.09375</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -469,7 +469,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>45946.10416666666</v>
+        <v>45947.10416666666</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>45946.11458333334</v>
+        <v>45947.11458333334</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>45946.125</v>
+        <v>45947.125</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>45946.13541666666</v>
+        <v>45947.13541666666</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>45946.14583333334</v>
+        <v>45947.14583333334</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>45946.15625</v>
+        <v>45947.15625</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>45946.16666666666</v>
+        <v>45947.16666666666</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>45946.17708333334</v>
+        <v>45947.17708333334</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>45946.1875</v>
+        <v>45947.1875</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>45946.19791666666</v>
+        <v>45947.19791666666</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>45946.20833333334</v>
+        <v>45947.20833333334</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>45946.21875</v>
+        <v>45947.21875</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>45946.22916666666</v>
+        <v>45947.22916666666</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>45946.23958333334</v>
+        <v>45947.23958333334</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>45946.25</v>
+        <v>45947.25</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>45946.26041666666</v>
+        <v>45947.26041666666</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>45946.27083333334</v>
+        <v>45947.27083333334</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>45946.28125</v>
+        <v>45947.28125</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -613,127 +613,127 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>45946.29166666666</v>
+        <v>45947.29166666666</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>45946.30208333334</v>
+        <v>45947.30208333334</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>45946.3125</v>
+        <v>45947.3125</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>45946.32291666666</v>
+        <v>45947.32291666666</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>45946.33333333334</v>
+        <v>45947.33333333334</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>289</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>45946.34375</v>
+        <v>45947.34375</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>421</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>45946.35416666666</v>
+        <v>45947.35416666666</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>541</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>45946.36458333334</v>
+        <v>45947.36458333334</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>654</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>45946.375</v>
+        <v>45947.375</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>761</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>45946.38541666666</v>
+        <v>45947.38541666666</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>828</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>45946.39583333334</v>
+        <v>45947.39583333334</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>916</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>45946.40625</v>
+        <v>45947.40625</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>982</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>45946.41666666666</v>
+        <v>45947.41666666666</v>
       </c>
       <c r="B41">
-        <v>759</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>45946.42708333334</v>
+        <v>45947.42708333334</v>
       </c>
       <c r="B42">
-        <v>789</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>45946.4375</v>
+        <v>45947.4375</v>
       </c>
       <c r="B43">
-        <v>846</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>45946.44791666666</v>
+        <v>45947.44791666666</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>45946.45833333334</v>
+        <v>45947.45833333334</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>45946.46875</v>
+        <v>45947.46875</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>45946.47916666666</v>
+        <v>45947.47916666666</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>45946.48958333334</v>
+        <v>45947.48958333334</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>45946.5</v>
+        <v>45947.5</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>45946.51041666666</v>
+        <v>45947.51041666666</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>45946.52083333334</v>
+        <v>45947.52083333334</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>45946.53125</v>
+        <v>45947.53125</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>45946.54166666666</v>
+        <v>45947.54166666666</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>45946.55208333334</v>
+        <v>45947.55208333334</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>45946.5625</v>
+        <v>45947.5625</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>45946.57291666666</v>
+        <v>45947.57291666666</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>45946.58333333334</v>
+        <v>45947.58333333334</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>45946.59375</v>
+        <v>45947.59375</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -853,7 +853,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>45946.60416666666</v>
+        <v>45947.60416666666</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>45946.61458333334</v>
+        <v>45947.61458333334</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>45946.625</v>
+        <v>45947.625</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>45946.63541666666</v>
+        <v>45947.63541666666</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>45946.64583333334</v>
+        <v>45947.64583333334</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>45946.65625</v>
+        <v>45947.65625</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>45946.66666666666</v>
+        <v>45947.66666666666</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>45946.67708333334</v>
+        <v>45947.67708333334</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>45946.6875</v>
+        <v>45947.6875</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>45946.69791666666</v>
+        <v>45947.69791666666</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>45946.70833333334</v>
+        <v>45947.70833333334</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>45946.71875</v>
+        <v>45947.71875</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>45946.72916666666</v>
+        <v>45947.72916666666</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>45946.73958333334</v>
+        <v>45947.73958333334</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>45946.75</v>
+        <v>45947.75</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>45946.76041666666</v>
+        <v>45947.76041666666</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>45946.77083333334</v>
+        <v>45947.77083333334</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2">
-        <v>45946.78125</v>
+        <v>45947.78125</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2">
-        <v>45946.79166666666</v>
+        <v>45947.79166666666</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2">
-        <v>45946.80208333334</v>
+        <v>45947.80208333334</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2">
-        <v>45946.8125</v>
+        <v>45947.8125</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2">
-        <v>45946.82291666666</v>
+        <v>45947.82291666666</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
-        <v>45946.83333333334</v>
+        <v>45947.83333333334</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2">
-        <v>45946.84375</v>
+        <v>45947.84375</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2">
-        <v>45946.85416666666</v>
+        <v>45947.85416666666</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2">
-        <v>45946.86458333334</v>
+        <v>45947.86458333334</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2">
-        <v>45946.875</v>
+        <v>45947.875</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2">
-        <v>45946.88541666666</v>
+        <v>45947.88541666666</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2">
-        <v>45946.89583333334</v>
+        <v>45947.89583333334</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2">
-        <v>45946.90625</v>
+        <v>45947.90625</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2">
-        <v>45946.91666666666</v>
+        <v>45947.91666666666</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2">
-        <v>45946.92708333334</v>
+        <v>45947.92708333334</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2">
-        <v>45946.9375</v>
+        <v>45947.9375</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2">
-        <v>45946.94791666666</v>
+        <v>45947.94791666666</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2">
-        <v>45946.95833333334</v>
+        <v>45947.95833333334</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2">
-        <v>45946.96875</v>
+        <v>45947.96875</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2">
-        <v>45946.97916666666</v>
+        <v>45947.97916666666</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2">
-        <v>45946.98958333334</v>
+        <v>45947.98958333334</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2">
-        <v>45947</v>
+        <v>45948</v>
       </c>
       <c r="B97">
         <v>0</v>

</xml_diff>

<commit_message>
Updating the model for MM&MV
</commit_message>
<xml_diff>
--- a/data_fetching/Entsoe/Actual_Production_Solar.xlsx
+++ b/data_fetching/Entsoe/Actual_Production_Solar.xlsx
@@ -397,7 +397,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>46069.01041666666</v>
+        <v>46070.01041666666</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -405,7 +405,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>46069.02083333334</v>
+        <v>46070.02083333334</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -413,7 +413,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>46069.03125</v>
+        <v>46070.03125</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -421,7 +421,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>46069.04166666666</v>
+        <v>46070.04166666666</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -429,7 +429,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>46069.05208333334</v>
+        <v>46070.05208333334</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -437,7 +437,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>46069.0625</v>
+        <v>46070.0625</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -445,7 +445,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>46069.07291666666</v>
+        <v>46070.07291666666</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>46069.08333333334</v>
+        <v>46070.08333333334</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>46069.09375</v>
+        <v>46070.09375</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -469,7 +469,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>46069.10416666666</v>
+        <v>46070.10416666666</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>46069.11458333334</v>
+        <v>46070.11458333334</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>46069.125</v>
+        <v>46070.125</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>46069.13541666666</v>
+        <v>46070.13541666666</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>46069.14583333334</v>
+        <v>46070.14583333334</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>46069.15625</v>
+        <v>46070.15625</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>46069.16666666666</v>
+        <v>46070.16666666666</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>46069.17708333334</v>
+        <v>46070.17708333334</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>46069.1875</v>
+        <v>46070.1875</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>46069.19791666666</v>
+        <v>46070.19791666666</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>46069.20833333334</v>
+        <v>46070.20833333334</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>46069.21875</v>
+        <v>46070.21875</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>46069.22916666666</v>
+        <v>46070.22916666666</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>46069.23958333334</v>
+        <v>46070.23958333334</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>46069.25</v>
+        <v>46070.25</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>46069.26041666666</v>
+        <v>46070.26041666666</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>46069.27083333334</v>
+        <v>46070.27083333334</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -605,31 +605,31 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>46069.28125</v>
+        <v>46070.28125</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>46069.29166666666</v>
+        <v>46070.29166666666</v>
       </c>
       <c r="B29">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>46069.30208333334</v>
+        <v>46070.30208333334</v>
       </c>
       <c r="B30">
-        <v>116</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>46069.3125</v>
+        <v>46070.3125</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>46069.32291666666</v>
+        <v>46070.32291666666</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>46069.33333333334</v>
+        <v>46070.33333333334</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>46069.34375</v>
+        <v>46070.34375</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>46069.35416666666</v>
+        <v>46070.35416666666</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>46069.36458333334</v>
+        <v>46070.36458333334</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>46069.375</v>
+        <v>46070.375</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>46069.38541666666</v>
+        <v>46070.38541666666</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>46069.39583333334</v>
+        <v>46070.39583333334</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>46069.40625</v>
+        <v>46070.40625</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>46069.41666666666</v>
+        <v>46070.41666666666</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>46069.42708333334</v>
+        <v>46070.42708333334</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>46069.4375</v>
+        <v>46070.4375</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>46069.44791666666</v>
+        <v>46070.44791666666</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>46069.45833333334</v>
+        <v>46070.45833333334</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>46069.46875</v>
+        <v>46070.46875</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>46069.47916666666</v>
+        <v>46070.47916666666</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>46069.48958333334</v>
+        <v>46070.48958333334</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>46069.5</v>
+        <v>46070.5</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>46069.51041666666</v>
+        <v>46070.51041666666</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>46069.52083333334</v>
+        <v>46070.52083333334</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>46069.53125</v>
+        <v>46070.53125</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>46069.54166666666</v>
+        <v>46070.54166666666</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>46069.55208333334</v>
+        <v>46070.55208333334</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>46069.5625</v>
+        <v>46070.5625</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>46069.57291666666</v>
+        <v>46070.57291666666</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>46069.58333333334</v>
+        <v>46070.58333333334</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>46069.59375</v>
+        <v>46070.59375</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -853,7 +853,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>46069.60416666666</v>
+        <v>46070.60416666666</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>46069.61458333334</v>
+        <v>46070.61458333334</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>46069.625</v>
+        <v>46070.625</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>46069.63541666666</v>
+        <v>46070.63541666666</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>46069.64583333334</v>
+        <v>46070.64583333334</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>46069.65625</v>
+        <v>46070.65625</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>46069.66666666666</v>
+        <v>46070.66666666666</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>46069.67708333334</v>
+        <v>46070.67708333334</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>46069.6875</v>
+        <v>46070.6875</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>46069.69791666666</v>
+        <v>46070.69791666666</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>46069.70833333334</v>
+        <v>46070.70833333334</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>46069.71875</v>
+        <v>46070.71875</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>46069.72916666666</v>
+        <v>46070.72916666666</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>46069.73958333334</v>
+        <v>46070.73958333334</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>46069.75</v>
+        <v>46070.75</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>46069.76041666666</v>
+        <v>46070.76041666666</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>46069.77083333334</v>
+        <v>46070.77083333334</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2">
-        <v>46069.78125</v>
+        <v>46070.78125</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2">
-        <v>46069.79166666666</v>
+        <v>46070.79166666666</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2">
-        <v>46069.80208333334</v>
+        <v>46070.80208333334</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2">
-        <v>46069.8125</v>
+        <v>46070.8125</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2">
-        <v>46069.82291666666</v>
+        <v>46070.82291666666</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
-        <v>46069.83333333334</v>
+        <v>46070.83333333334</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2">
-        <v>46069.84375</v>
+        <v>46070.84375</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2">
-        <v>46069.85416666666</v>
+        <v>46070.85416666666</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2">
-        <v>46069.86458333334</v>
+        <v>46070.86458333334</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2">
-        <v>46069.875</v>
+        <v>46070.875</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2">
-        <v>46069.88541666666</v>
+        <v>46070.88541666666</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2">
-        <v>46069.89583333334</v>
+        <v>46070.89583333334</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2">
-        <v>46069.90625</v>
+        <v>46070.90625</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2">
-        <v>46069.91666666666</v>
+        <v>46070.91666666666</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2">
-        <v>46069.92708333334</v>
+        <v>46070.92708333334</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2">
-        <v>46069.9375</v>
+        <v>46070.9375</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2">
-        <v>46069.94791666666</v>
+        <v>46070.94791666666</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2">
-        <v>46069.95833333334</v>
+        <v>46070.95833333334</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2">
-        <v>46069.96875</v>
+        <v>46070.96875</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2">
-        <v>46069.97916666666</v>
+        <v>46070.97916666666</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2">
-        <v>46069.98958333334</v>
+        <v>46070.98958333334</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2">
-        <v>46070</v>
+        <v>46071</v>
       </c>
       <c r="B97">
         <v>0</v>

</xml_diff>